<commit_message>
Added Statement Description as top line item and fixed some columns
</commit_message>
<xml_diff>
--- a/CCPPA Form.xlsx
+++ b/CCPPA Form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan.green\PPA project\Monday_PPA_Workflow_Enhancer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2BAF52-66D1-4652-9791-FA94B7128B5B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5936509-6595-4258-A64E-17FD79CE2E70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11865" windowHeight="6315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -803,7 +803,7 @@
     <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -997,14 +997,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="43" fontId="20" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="43" fontId="20" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="43" fontId="20" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -1029,229 +1021,233 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="43" fontId="20" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -1602,7 +1598,7 @@
   <dimension ref="A1:Z46"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="M41" sqref="M41"/>
+      <selection activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1631,96 +1627,96 @@
     <row r="1" spans="1:26" ht="22.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
       <c r="B1" s="9"/>
-      <c r="C1" s="122" t="s">
+      <c r="C1" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="123"/>
-      <c r="K1" s="123"/>
-      <c r="L1" s="123"/>
-      <c r="M1" s="123"/>
-      <c r="N1" s="124"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="89"/>
+      <c r="L1" s="89"/>
+      <c r="M1" s="89"/>
+      <c r="N1" s="90"/>
       <c r="P1" s="11"/>
     </row>
     <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8"/>
       <c r="B2" s="13"/>
-      <c r="C2" s="125" t="s">
+      <c r="C2" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="126"/>
-      <c r="E2" s="126"/>
-      <c r="F2" s="126"/>
-      <c r="G2" s="126"/>
-      <c r="H2" s="126"/>
-      <c r="I2" s="126"/>
-      <c r="J2" s="126"/>
-      <c r="K2" s="126"/>
-      <c r="L2" s="126"/>
-      <c r="M2" s="126"/>
-      <c r="N2" s="127"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="93"/>
       <c r="P2" s="11"/>
     </row>
     <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8"/>
       <c r="B3" s="13"/>
-      <c r="C3" s="128" t="s">
+      <c r="C3" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="129"/>
-      <c r="E3" s="129"/>
-      <c r="F3" s="129"/>
-      <c r="G3" s="129"/>
-      <c r="H3" s="129"/>
-      <c r="I3" s="129"/>
-      <c r="J3" s="129"/>
-      <c r="K3" s="129"/>
-      <c r="L3" s="129"/>
-      <c r="M3" s="129"/>
-      <c r="N3" s="130"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="95"/>
+      <c r="L3" s="95"/>
+      <c r="M3" s="95"/>
+      <c r="N3" s="96"/>
       <c r="P3" s="11"/>
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="13"/>
-      <c r="C4" s="128" t="s">
+      <c r="C4" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="129"/>
-      <c r="E4" s="129"/>
-      <c r="F4" s="129"/>
-      <c r="G4" s="129"/>
-      <c r="H4" s="129"/>
-      <c r="I4" s="129"/>
-      <c r="J4" s="129"/>
-      <c r="K4" s="129"/>
-      <c r="L4" s="129"/>
-      <c r="M4" s="129"/>
-      <c r="N4" s="130"/>
+      <c r="D4" s="95"/>
+      <c r="E4" s="95"/>
+      <c r="F4" s="95"/>
+      <c r="G4" s="95"/>
+      <c r="H4" s="95"/>
+      <c r="I4" s="95"/>
+      <c r="J4" s="95"/>
+      <c r="K4" s="95"/>
+      <c r="L4" s="95"/>
+      <c r="M4" s="95"/>
+      <c r="N4" s="96"/>
       <c r="P4" s="11"/>
     </row>
     <row r="5" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8"/>
       <c r="B5" s="13"/>
-      <c r="C5" s="128" t="s">
+      <c r="C5" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="129"/>
-      <c r="E5" s="129"/>
-      <c r="F5" s="129"/>
-      <c r="G5" s="129"/>
-      <c r="H5" s="129"/>
-      <c r="I5" s="129"/>
-      <c r="J5" s="129"/>
-      <c r="K5" s="129"/>
-      <c r="L5" s="129"/>
-      <c r="M5" s="129"/>
-      <c r="N5" s="130"/>
+      <c r="D5" s="95"/>
+      <c r="E5" s="95"/>
+      <c r="F5" s="95"/>
+      <c r="G5" s="95"/>
+      <c r="H5" s="95"/>
+      <c r="I5" s="95"/>
+      <c r="J5" s="95"/>
+      <c r="K5" s="95"/>
+      <c r="L5" s="95"/>
+      <c r="M5" s="95"/>
+      <c r="N5" s="96"/>
       <c r="P5" s="11"/>
     </row>
     <row r="6" spans="1:26" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1762,25 +1758,25 @@
       <c r="P7" s="11"/>
     </row>
     <row r="8" spans="1:26" s="18" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="131" t="s">
+      <c r="B8" s="97" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="131"/>
-      <c r="D8" s="131"/>
-      <c r="E8" s="132"/>
-      <c r="F8" s="132"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="98"/>
+      <c r="F8" s="98"/>
       <c r="G8" s="19"/>
       <c r="H8" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="133"/>
-      <c r="J8" s="133"/>
-      <c r="K8" s="133"/>
-      <c r="L8" s="133"/>
-      <c r="M8" s="134" t="s">
+      <c r="I8" s="99"/>
+      <c r="J8" s="99"/>
+      <c r="K8" s="99"/>
+      <c r="L8" s="99"/>
+      <c r="M8" s="100" t="s">
         <v>21</v>
       </c>
-      <c r="N8" s="134"/>
+      <c r="N8" s="100"/>
       <c r="O8" s="60" t="s">
         <v>10</v>
       </c>
@@ -1814,23 +1810,23 @@
       <c r="P9" s="11"/>
     </row>
     <row r="10" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="135" t="s">
+      <c r="B10" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="136"/>
-      <c r="D10" s="136"/>
-      <c r="E10" s="136"/>
-      <c r="F10" s="136"/>
-      <c r="G10" s="137"/>
-      <c r="H10" s="138"/>
+      <c r="C10" s="102"/>
+      <c r="D10" s="102"/>
+      <c r="E10" s="102"/>
+      <c r="F10" s="102"/>
+      <c r="G10" s="103"/>
+      <c r="H10" s="104"/>
       <c r="I10" s="22"/>
       <c r="J10" s="9"/>
       <c r="K10" s="23"/>
-      <c r="L10" s="135" t="s">
+      <c r="L10" s="101" t="s">
         <v>39</v>
       </c>
-      <c r="M10" s="136"/>
-      <c r="N10" s="136"/>
+      <c r="M10" s="102"/>
+      <c r="N10" s="102"/>
       <c r="O10" s="63"/>
       <c r="P10" s="24"/>
       <c r="Q10" s="25"/>
@@ -1841,49 +1837,49 @@
       <c r="V10" s="25"/>
     </row>
     <row r="11" spans="1:26" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="139" t="s">
+      <c r="B11" s="105" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="140"/>
-      <c r="D11" s="140"/>
-      <c r="E11" s="140"/>
-      <c r="F11" s="140"/>
-      <c r="G11" s="140"/>
-      <c r="H11" s="141"/>
+      <c r="C11" s="106"/>
+      <c r="D11" s="106"/>
+      <c r="E11" s="106"/>
+      <c r="F11" s="106"/>
+      <c r="G11" s="106"/>
+      <c r="H11" s="107"/>
       <c r="I11" s="26"/>
       <c r="J11" s="27"/>
       <c r="K11" s="26"/>
-      <c r="L11" s="142" t="s">
+      <c r="L11" s="108" t="s">
         <v>42</v>
       </c>
-      <c r="M11" s="143"/>
-      <c r="N11" s="143"/>
-      <c r="O11" s="144"/>
+      <c r="M11" s="109"/>
+      <c r="N11" s="109"/>
+      <c r="O11" s="110"/>
       <c r="P11" s="28"/>
-      <c r="Q11" s="110"/>
-      <c r="R11" s="110"/>
-      <c r="S11" s="110"/>
-      <c r="T11" s="110"/>
-      <c r="U11" s="110"/>
-      <c r="V11" s="110"/>
+      <c r="Q11" s="87"/>
+      <c r="R11" s="87"/>
+      <c r="S11" s="87"/>
+      <c r="T11" s="87"/>
+      <c r="U11" s="87"/>
+      <c r="V11" s="87"/>
     </row>
     <row r="12" spans="1:26" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="116"/>
-      <c r="C12" s="117"/>
-      <c r="D12" s="117"/>
-      <c r="E12" s="117"/>
-      <c r="F12" s="117"/>
-      <c r="G12" s="117"/>
-      <c r="H12" s="118"/>
+      <c r="B12" s="112"/>
+      <c r="C12" s="113"/>
+      <c r="D12" s="113"/>
+      <c r="E12" s="113"/>
+      <c r="F12" s="113"/>
+      <c r="G12" s="113"/>
+      <c r="H12" s="114"/>
       <c r="I12" s="26"/>
       <c r="J12" s="27"/>
       <c r="K12" s="26"/>
-      <c r="L12" s="119" t="s">
+      <c r="L12" s="115" t="s">
         <v>43</v>
       </c>
-      <c r="M12" s="120"/>
-      <c r="N12" s="120"/>
-      <c r="O12" s="121"/>
+      <c r="M12" s="116"/>
+      <c r="N12" s="116"/>
+      <c r="O12" s="117"/>
       <c r="P12" s="28"/>
       <c r="Q12" s="62"/>
       <c r="R12" s="62"/>
@@ -1893,22 +1889,22 @@
       <c r="V12" s="62"/>
     </row>
     <row r="13" spans="1:26" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="116"/>
-      <c r="C13" s="117"/>
-      <c r="D13" s="117"/>
-      <c r="E13" s="117"/>
-      <c r="F13" s="117"/>
-      <c r="G13" s="117"/>
-      <c r="H13" s="118"/>
+      <c r="B13" s="112"/>
+      <c r="C13" s="113"/>
+      <c r="D13" s="113"/>
+      <c r="E13" s="113"/>
+      <c r="F13" s="113"/>
+      <c r="G13" s="113"/>
+      <c r="H13" s="114"/>
       <c r="I13" s="26"/>
       <c r="J13" s="27"/>
       <c r="K13" s="26"/>
-      <c r="L13" s="119" t="s">
+      <c r="L13" s="115" t="s">
         <v>44</v>
       </c>
-      <c r="M13" s="120"/>
-      <c r="N13" s="120"/>
-      <c r="O13" s="121"/>
+      <c r="M13" s="116"/>
+      <c r="N13" s="116"/>
+      <c r="O13" s="117"/>
       <c r="P13" s="28"/>
       <c r="Q13" s="62"/>
       <c r="R13" s="62"/>
@@ -1918,66 +1914,66 @@
       <c r="V13" s="62"/>
     </row>
     <row r="14" spans="1:26" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="116"/>
-      <c r="C14" s="117"/>
-      <c r="D14" s="117"/>
-      <c r="E14" s="117"/>
-      <c r="F14" s="117"/>
-      <c r="G14" s="117"/>
-      <c r="H14" s="118"/>
+      <c r="B14" s="112"/>
+      <c r="C14" s="113"/>
+      <c r="D14" s="113"/>
+      <c r="E14" s="113"/>
+      <c r="F14" s="113"/>
+      <c r="G14" s="113"/>
+      <c r="H14" s="114"/>
       <c r="I14" s="26"/>
       <c r="J14" s="27"/>
       <c r="K14" s="26"/>
-      <c r="L14" s="116"/>
-      <c r="M14" s="117"/>
-      <c r="N14" s="117"/>
-      <c r="O14" s="118"/>
+      <c r="L14" s="112"/>
+      <c r="M14" s="113"/>
+      <c r="N14" s="113"/>
+      <c r="O14" s="114"/>
       <c r="P14" s="28"/>
-      <c r="Q14" s="110"/>
-      <c r="R14" s="110"/>
-      <c r="S14" s="110"/>
-      <c r="T14" s="110"/>
-      <c r="U14" s="110"/>
-      <c r="V14" s="110"/>
+      <c r="Q14" s="87"/>
+      <c r="R14" s="87"/>
+      <c r="S14" s="87"/>
+      <c r="T14" s="87"/>
+      <c r="U14" s="87"/>
+      <c r="V14" s="87"/>
     </row>
     <row r="15" spans="1:26" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="111"/>
-      <c r="C15" s="112"/>
-      <c r="D15" s="112"/>
-      <c r="E15" s="112"/>
-      <c r="F15" s="112"/>
-      <c r="G15" s="112"/>
-      <c r="H15" s="113"/>
+      <c r="B15" s="118"/>
+      <c r="C15" s="119"/>
+      <c r="D15" s="119"/>
+      <c r="E15" s="119"/>
+      <c r="F15" s="119"/>
+      <c r="G15" s="119"/>
+      <c r="H15" s="120"/>
       <c r="I15" s="26"/>
       <c r="J15" s="27"/>
       <c r="K15" s="26"/>
-      <c r="L15" s="111"/>
-      <c r="M15" s="112"/>
-      <c r="N15" s="112"/>
-      <c r="O15" s="113"/>
+      <c r="L15" s="118"/>
+      <c r="M15" s="119"/>
+      <c r="N15" s="119"/>
+      <c r="O15" s="120"/>
       <c r="P15" s="28"/>
-      <c r="Q15" s="110"/>
-      <c r="R15" s="110"/>
-      <c r="S15" s="110"/>
-      <c r="T15" s="110"/>
-      <c r="U15" s="110"/>
-      <c r="V15" s="110"/>
+      <c r="Q15" s="87"/>
+      <c r="R15" s="87"/>
+      <c r="S15" s="87"/>
+      <c r="T15" s="87"/>
+      <c r="U15" s="87"/>
+      <c r="V15" s="87"/>
     </row>
     <row r="16" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="114"/>
-      <c r="D16" s="114"/>
-      <c r="E16" s="114"/>
-      <c r="F16" s="114"/>
-      <c r="G16" s="114"/>
-      <c r="H16" s="114"/>
-      <c r="I16" s="114"/>
-      <c r="J16" s="114"/>
-      <c r="K16" s="114"/>
-      <c r="L16" s="114"/>
+      <c r="C16" s="121"/>
+      <c r="D16" s="121"/>
+      <c r="E16" s="121"/>
+      <c r="F16" s="121"/>
+      <c r="G16" s="121"/>
+      <c r="H16" s="121"/>
+      <c r="I16" s="121"/>
+      <c r="J16" s="121"/>
+      <c r="K16" s="121"/>
+      <c r="L16" s="121"/>
       <c r="M16" s="9"/>
       <c r="N16" s="30"/>
       <c r="O16" s="31"/>
@@ -1988,16 +1984,16 @@
       <c r="B17" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="115"/>
-      <c r="D17" s="115"/>
-      <c r="E17" s="115"/>
-      <c r="F17" s="115"/>
-      <c r="G17" s="115"/>
-      <c r="H17" s="115"/>
-      <c r="I17" s="115"/>
-      <c r="J17" s="115"/>
-      <c r="K17" s="115"/>
-      <c r="L17" s="115"/>
+      <c r="C17" s="111"/>
+      <c r="D17" s="111"/>
+      <c r="E17" s="111"/>
+      <c r="F17" s="111"/>
+      <c r="G17" s="111"/>
+      <c r="H17" s="111"/>
+      <c r="I17" s="111"/>
+      <c r="J17" s="111"/>
+      <c r="K17" s="111"/>
+      <c r="L17" s="111"/>
       <c r="M17" s="9"/>
       <c r="N17" s="30"/>
       <c r="O17" s="31"/>
@@ -2009,43 +2005,43 @@
       <c r="C18" s="33"/>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
-      <c r="F18" s="101"/>
-      <c r="G18" s="101"/>
-      <c r="H18" s="101"/>
-      <c r="I18" s="101"/>
-      <c r="J18" s="101"/>
-      <c r="K18" s="101"/>
-      <c r="L18" s="101"/>
-      <c r="M18" s="101"/>
-      <c r="N18" s="101"/>
-      <c r="O18" s="101"/>
+      <c r="F18" s="122"/>
+      <c r="G18" s="122"/>
+      <c r="H18" s="122"/>
+      <c r="I18" s="122"/>
+      <c r="J18" s="122"/>
+      <c r="K18" s="122"/>
+      <c r="L18" s="122"/>
+      <c r="M18" s="122"/>
+      <c r="N18" s="122"/>
+      <c r="O18" s="122"/>
       <c r="P18" s="11"/>
     </row>
     <row r="19" spans="1:19" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="82" t="s">
+      <c r="B19" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="102">
+      <c r="C19" s="123">
         <f ca="1">TODAY()</f>
-        <v>45922</v>
-      </c>
-      <c r="D19" s="102"/>
-      <c r="E19" s="103"/>
-      <c r="F19" s="81" t="s">
+        <v>45925</v>
+      </c>
+      <c r="D19" s="123"/>
+      <c r="E19" s="124"/>
+      <c r="F19" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="G19" s="104"/>
-      <c r="H19" s="104"/>
-      <c r="I19" s="105"/>
-      <c r="J19" s="106" t="s">
+      <c r="G19" s="125"/>
+      <c r="H19" s="125"/>
+      <c r="I19" s="126"/>
+      <c r="J19" s="127" t="s">
         <v>20</v>
       </c>
-      <c r="K19" s="107"/>
-      <c r="L19" s="108" t="s">
+      <c r="K19" s="128"/>
+      <c r="L19" s="129" t="s">
         <v>41</v>
       </c>
-      <c r="M19" s="109"/>
-      <c r="N19" s="80" t="s">
+      <c r="M19" s="130"/>
+      <c r="N19" s="78" t="s">
         <v>35</v>
       </c>
       <c r="O19" s="51" t="s">
@@ -2054,24 +2050,24 @@
       <c r="P19" s="34"/>
     </row>
     <row r="20" spans="1:19" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="90" t="s">
+      <c r="B20" s="131" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="91"/>
-      <c r="D20" s="92"/>
-      <c r="E20" s="93"/>
+      <c r="C20" s="132"/>
+      <c r="D20" s="133"/>
+      <c r="E20" s="134"/>
       <c r="F20" s="35" t="s">
         <v>3</v>
       </c>
       <c r="G20" s="35"/>
-      <c r="H20" s="94"/>
-      <c r="I20" s="94"/>
-      <c r="J20" s="95"/>
-      <c r="K20" s="96"/>
-      <c r="L20" s="96"/>
-      <c r="M20" s="96"/>
-      <c r="N20" s="96"/>
-      <c r="O20" s="97"/>
+      <c r="H20" s="135"/>
+      <c r="I20" s="135"/>
+      <c r="J20" s="136"/>
+      <c r="K20" s="137"/>
+      <c r="L20" s="137"/>
+      <c r="M20" s="137"/>
+      <c r="N20" s="137"/>
+      <c r="O20" s="138"/>
       <c r="P20" s="36"/>
     </row>
     <row r="21" spans="1:19" ht="8.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2099,18 +2095,18 @@
       <c r="B22" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="98" t="s">
+      <c r="C22" s="139" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="99"/>
-      <c r="E22" s="99"/>
-      <c r="F22" s="99"/>
-      <c r="G22" s="99"/>
-      <c r="H22" s="99"/>
-      <c r="I22" s="99"/>
-      <c r="J22" s="99"/>
-      <c r="K22" s="99"/>
-      <c r="L22" s="100"/>
+      <c r="D22" s="140"/>
+      <c r="E22" s="140"/>
+      <c r="F22" s="140"/>
+      <c r="G22" s="140"/>
+      <c r="H22" s="140"/>
+      <c r="I22" s="140"/>
+      <c r="J22" s="140"/>
+      <c r="K22" s="140"/>
+      <c r="L22" s="141"/>
       <c r="M22" s="41" t="s">
         <v>23</v>
       </c>
@@ -2128,16 +2124,16 @@
     <row r="23" spans="1:19" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
       <c r="B23" s="64"/>
-      <c r="C23" s="145"/>
-      <c r="D23" s="146"/>
-      <c r="E23" s="146"/>
-      <c r="F23" s="146"/>
-      <c r="G23" s="146"/>
-      <c r="H23" s="146"/>
-      <c r="I23" s="146"/>
-      <c r="J23" s="146"/>
-      <c r="K23" s="146"/>
-      <c r="L23" s="147"/>
+      <c r="C23" s="84"/>
+      <c r="D23" s="85"/>
+      <c r="E23" s="85"/>
+      <c r="F23" s="85"/>
+      <c r="G23" s="85"/>
+      <c r="H23" s="85"/>
+      <c r="I23" s="85"/>
+      <c r="J23" s="85"/>
+      <c r="K23" s="85"/>
+      <c r="L23" s="86"/>
       <c r="M23" s="65"/>
       <c r="N23" s="66"/>
       <c r="O23" s="67">
@@ -2152,16 +2148,16 @@
     <row r="24" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
       <c r="B24" s="68"/>
-      <c r="C24" s="87"/>
-      <c r="D24" s="88"/>
-      <c r="E24" s="88"/>
-      <c r="F24" s="88"/>
-      <c r="G24" s="88"/>
-      <c r="H24" s="88"/>
-      <c r="I24" s="88"/>
-      <c r="J24" s="88"/>
-      <c r="K24" s="88"/>
-      <c r="L24" s="89"/>
+      <c r="C24" s="81"/>
+      <c r="D24" s="82"/>
+      <c r="E24" s="82"/>
+      <c r="F24" s="82"/>
+      <c r="G24" s="82"/>
+      <c r="H24" s="82"/>
+      <c r="I24" s="82"/>
+      <c r="J24" s="82"/>
+      <c r="K24" s="82"/>
+      <c r="L24" s="83"/>
       <c r="M24" s="69"/>
       <c r="N24" s="70"/>
       <c r="O24" s="71">
@@ -2176,16 +2172,16 @@
     <row r="25" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9"/>
       <c r="B25" s="64"/>
-      <c r="C25" s="87"/>
-      <c r="D25" s="88"/>
-      <c r="E25" s="88"/>
-      <c r="F25" s="88"/>
-      <c r="G25" s="88"/>
-      <c r="H25" s="88"/>
-      <c r="I25" s="88"/>
-      <c r="J25" s="88"/>
-      <c r="K25" s="88"/>
-      <c r="L25" s="89"/>
+      <c r="C25" s="81"/>
+      <c r="D25" s="82"/>
+      <c r="E25" s="82"/>
+      <c r="F25" s="82"/>
+      <c r="G25" s="82"/>
+      <c r="H25" s="82"/>
+      <c r="I25" s="82"/>
+      <c r="J25" s="82"/>
+      <c r="K25" s="82"/>
+      <c r="L25" s="83"/>
       <c r="M25" s="69"/>
       <c r="N25" s="70"/>
       <c r="O25" s="71">
@@ -2202,16 +2198,16 @@
         <v>1</v>
       </c>
       <c r="B26" s="68"/>
-      <c r="C26" s="87"/>
-      <c r="D26" s="88"/>
-      <c r="E26" s="88"/>
-      <c r="F26" s="88"/>
-      <c r="G26" s="88"/>
-      <c r="H26" s="88"/>
-      <c r="I26" s="88"/>
-      <c r="J26" s="88"/>
-      <c r="K26" s="88"/>
-      <c r="L26" s="89"/>
+      <c r="C26" s="81"/>
+      <c r="D26" s="82"/>
+      <c r="E26" s="82"/>
+      <c r="F26" s="82"/>
+      <c r="G26" s="82"/>
+      <c r="H26" s="82"/>
+      <c r="I26" s="82"/>
+      <c r="J26" s="82"/>
+      <c r="K26" s="82"/>
+      <c r="L26" s="83"/>
       <c r="M26" s="69"/>
       <c r="N26" s="70"/>
       <c r="O26" s="71">
@@ -2226,16 +2222,16 @@
     <row r="27" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="9"/>
       <c r="B27" s="68"/>
-      <c r="C27" s="87"/>
-      <c r="D27" s="88"/>
-      <c r="E27" s="88"/>
-      <c r="F27" s="88"/>
-      <c r="G27" s="88"/>
-      <c r="H27" s="88"/>
-      <c r="I27" s="88"/>
-      <c r="J27" s="88"/>
-      <c r="K27" s="88"/>
-      <c r="L27" s="89"/>
+      <c r="C27" s="81"/>
+      <c r="D27" s="82"/>
+      <c r="E27" s="82"/>
+      <c r="F27" s="82"/>
+      <c r="G27" s="82"/>
+      <c r="H27" s="82"/>
+      <c r="I27" s="82"/>
+      <c r="J27" s="82"/>
+      <c r="K27" s="82"/>
+      <c r="L27" s="83"/>
       <c r="M27" s="69"/>
       <c r="N27" s="70"/>
       <c r="O27" s="71">
@@ -2249,16 +2245,16 @@
     <row r="28" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="9"/>
       <c r="B28" s="68"/>
-      <c r="C28" s="87"/>
-      <c r="D28" s="88"/>
-      <c r="E28" s="88"/>
-      <c r="F28" s="88"/>
-      <c r="G28" s="88"/>
-      <c r="H28" s="88"/>
-      <c r="I28" s="88"/>
-      <c r="J28" s="88"/>
-      <c r="K28" s="88"/>
-      <c r="L28" s="89"/>
+      <c r="C28" s="81"/>
+      <c r="D28" s="82"/>
+      <c r="E28" s="82"/>
+      <c r="F28" s="82"/>
+      <c r="G28" s="82"/>
+      <c r="H28" s="82"/>
+      <c r="I28" s="82"/>
+      <c r="J28" s="82"/>
+      <c r="K28" s="82"/>
+      <c r="L28" s="83"/>
       <c r="M28" s="69"/>
       <c r="N28" s="70"/>
       <c r="O28" s="71">
@@ -2270,16 +2266,16 @@
     <row r="29" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9"/>
       <c r="B29" s="68"/>
-      <c r="C29" s="87"/>
-      <c r="D29" s="88"/>
-      <c r="E29" s="88"/>
-      <c r="F29" s="88"/>
-      <c r="G29" s="88"/>
-      <c r="H29" s="88"/>
-      <c r="I29" s="88"/>
-      <c r="J29" s="88"/>
-      <c r="K29" s="88"/>
-      <c r="L29" s="89"/>
+      <c r="C29" s="81"/>
+      <c r="D29" s="82"/>
+      <c r="E29" s="82"/>
+      <c r="F29" s="82"/>
+      <c r="G29" s="82"/>
+      <c r="H29" s="82"/>
+      <c r="I29" s="82"/>
+      <c r="J29" s="82"/>
+      <c r="K29" s="82"/>
+      <c r="L29" s="83"/>
       <c r="M29" s="69"/>
       <c r="N29" s="70"/>
       <c r="O29" s="71">
@@ -2291,16 +2287,16 @@
     <row r="30" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="9"/>
       <c r="B30" s="68"/>
-      <c r="C30" s="87"/>
-      <c r="D30" s="88"/>
-      <c r="E30" s="88"/>
-      <c r="F30" s="88"/>
-      <c r="G30" s="88"/>
-      <c r="H30" s="88"/>
-      <c r="I30" s="88"/>
-      <c r="J30" s="88"/>
-      <c r="K30" s="88"/>
-      <c r="L30" s="89"/>
+      <c r="C30" s="81"/>
+      <c r="D30" s="82"/>
+      <c r="E30" s="82"/>
+      <c r="F30" s="82"/>
+      <c r="G30" s="82"/>
+      <c r="H30" s="82"/>
+      <c r="I30" s="82"/>
+      <c r="J30" s="82"/>
+      <c r="K30" s="82"/>
+      <c r="L30" s="83"/>
       <c r="M30" s="69"/>
       <c r="N30" s="72"/>
       <c r="O30" s="71">
@@ -2312,18 +2308,18 @@
     <row r="31" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
       <c r="B31" s="68"/>
-      <c r="C31" s="87"/>
-      <c r="D31" s="88"/>
-      <c r="E31" s="88"/>
-      <c r="F31" s="88"/>
-      <c r="G31" s="88"/>
-      <c r="H31" s="88"/>
-      <c r="I31" s="88"/>
-      <c r="J31" s="88"/>
-      <c r="K31" s="88"/>
-      <c r="L31" s="89"/>
+      <c r="C31" s="81"/>
+      <c r="D31" s="82"/>
+      <c r="E31" s="82"/>
+      <c r="F31" s="82"/>
+      <c r="G31" s="82"/>
+      <c r="H31" s="82"/>
+      <c r="I31" s="82"/>
+      <c r="J31" s="82"/>
+      <c r="K31" s="82"/>
+      <c r="L31" s="83"/>
       <c r="M31" s="69"/>
-      <c r="N31" s="73"/>
+      <c r="N31" s="72"/>
       <c r="O31" s="71">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2333,18 +2329,18 @@
     <row r="32" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
       <c r="B32" s="68"/>
-      <c r="C32" s="87"/>
-      <c r="D32" s="88"/>
-      <c r="E32" s="88"/>
-      <c r="F32" s="88"/>
-      <c r="G32" s="88"/>
-      <c r="H32" s="88"/>
-      <c r="I32" s="88"/>
-      <c r="J32" s="88"/>
-      <c r="K32" s="88"/>
-      <c r="L32" s="89"/>
+      <c r="C32" s="81"/>
+      <c r="D32" s="82"/>
+      <c r="E32" s="82"/>
+      <c r="F32" s="82"/>
+      <c r="G32" s="82"/>
+      <c r="H32" s="82"/>
+      <c r="I32" s="82"/>
+      <c r="J32" s="82"/>
+      <c r="K32" s="82"/>
+      <c r="L32" s="83"/>
       <c r="M32" s="69"/>
-      <c r="N32" s="73"/>
+      <c r="N32" s="72"/>
       <c r="O32" s="71">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2354,18 +2350,18 @@
     <row r="33" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
       <c r="B33" s="68"/>
-      <c r="C33" s="87"/>
-      <c r="D33" s="88"/>
-      <c r="E33" s="88"/>
-      <c r="F33" s="88"/>
-      <c r="G33" s="88"/>
-      <c r="H33" s="88"/>
-      <c r="I33" s="88"/>
-      <c r="J33" s="88"/>
-      <c r="K33" s="88"/>
-      <c r="L33" s="89"/>
+      <c r="C33" s="81"/>
+      <c r="D33" s="82"/>
+      <c r="E33" s="82"/>
+      <c r="F33" s="82"/>
+      <c r="G33" s="82"/>
+      <c r="H33" s="82"/>
+      <c r="I33" s="82"/>
+      <c r="J33" s="82"/>
+      <c r="K33" s="82"/>
+      <c r="L33" s="83"/>
       <c r="M33" s="69"/>
-      <c r="N33" s="73"/>
+      <c r="N33" s="72"/>
       <c r="O33" s="71">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2375,18 +2371,18 @@
     <row r="34" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>
       <c r="B34" s="68"/>
-      <c r="C34" s="87"/>
-      <c r="D34" s="88"/>
-      <c r="E34" s="88"/>
-      <c r="F34" s="88"/>
-      <c r="G34" s="88"/>
-      <c r="H34" s="88"/>
-      <c r="I34" s="88"/>
-      <c r="J34" s="88"/>
-      <c r="K34" s="88"/>
-      <c r="L34" s="89"/>
+      <c r="C34" s="81"/>
+      <c r="D34" s="82"/>
+      <c r="E34" s="82"/>
+      <c r="F34" s="82"/>
+      <c r="G34" s="82"/>
+      <c r="H34" s="82"/>
+      <c r="I34" s="82"/>
+      <c r="J34" s="82"/>
+      <c r="K34" s="82"/>
+      <c r="L34" s="83"/>
       <c r="M34" s="69"/>
-      <c r="N34" s="74"/>
+      <c r="N34" s="146"/>
       <c r="O34" s="71">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2396,18 +2392,18 @@
     <row r="35" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
       <c r="B35" s="68"/>
-      <c r="C35" s="87"/>
-      <c r="D35" s="88"/>
-      <c r="E35" s="88"/>
-      <c r="F35" s="88"/>
-      <c r="G35" s="88"/>
-      <c r="H35" s="88"/>
-      <c r="I35" s="88"/>
-      <c r="J35" s="88"/>
-      <c r="K35" s="88"/>
-      <c r="L35" s="89"/>
+      <c r="C35" s="81"/>
+      <c r="D35" s="82"/>
+      <c r="E35" s="82"/>
+      <c r="F35" s="82"/>
+      <c r="G35" s="82"/>
+      <c r="H35" s="82"/>
+      <c r="I35" s="82"/>
+      <c r="J35" s="82"/>
+      <c r="K35" s="82"/>
+      <c r="L35" s="83"/>
       <c r="M35" s="69"/>
-      <c r="N35" s="74"/>
+      <c r="N35" s="146"/>
       <c r="O35" s="71">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2417,18 +2413,18 @@
     <row r="36" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9"/>
       <c r="B36" s="68"/>
-      <c r="C36" s="87"/>
-      <c r="D36" s="88"/>
-      <c r="E36" s="88"/>
-      <c r="F36" s="88"/>
-      <c r="G36" s="88"/>
-      <c r="H36" s="88"/>
-      <c r="I36" s="88"/>
-      <c r="J36" s="88"/>
-      <c r="K36" s="88"/>
-      <c r="L36" s="89"/>
+      <c r="C36" s="81"/>
+      <c r="D36" s="82"/>
+      <c r="E36" s="82"/>
+      <c r="F36" s="82"/>
+      <c r="G36" s="82"/>
+      <c r="H36" s="82"/>
+      <c r="I36" s="82"/>
+      <c r="J36" s="82"/>
+      <c r="K36" s="82"/>
+      <c r="L36" s="83"/>
       <c r="M36" s="69"/>
-      <c r="N36" s="74"/>
+      <c r="N36" s="146"/>
       <c r="O36" s="71">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2438,18 +2434,18 @@
     <row r="37" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="9"/>
       <c r="B37" s="68"/>
-      <c r="C37" s="87"/>
-      <c r="D37" s="88"/>
-      <c r="E37" s="88"/>
-      <c r="F37" s="88"/>
-      <c r="G37" s="88"/>
-      <c r="H37" s="88"/>
-      <c r="I37" s="88"/>
-      <c r="J37" s="88"/>
-      <c r="K37" s="88"/>
-      <c r="L37" s="89"/>
+      <c r="C37" s="81"/>
+      <c r="D37" s="82"/>
+      <c r="E37" s="82"/>
+      <c r="F37" s="82"/>
+      <c r="G37" s="82"/>
+      <c r="H37" s="82"/>
+      <c r="I37" s="82"/>
+      <c r="J37" s="82"/>
+      <c r="K37" s="82"/>
+      <c r="L37" s="83"/>
       <c r="M37" s="69"/>
-      <c r="N37" s="74"/>
+      <c r="N37" s="146"/>
       <c r="O37" s="71">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2459,18 +2455,18 @@
     <row r="38" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
       <c r="B38" s="68"/>
-      <c r="C38" s="87"/>
-      <c r="D38" s="88"/>
-      <c r="E38" s="88"/>
-      <c r="F38" s="88"/>
-      <c r="G38" s="88"/>
-      <c r="H38" s="88"/>
-      <c r="I38" s="88"/>
-      <c r="J38" s="88"/>
-      <c r="K38" s="88"/>
-      <c r="L38" s="89"/>
+      <c r="C38" s="81"/>
+      <c r="D38" s="82"/>
+      <c r="E38" s="82"/>
+      <c r="F38" s="82"/>
+      <c r="G38" s="82"/>
+      <c r="H38" s="82"/>
+      <c r="I38" s="82"/>
+      <c r="J38" s="82"/>
+      <c r="K38" s="82"/>
+      <c r="L38" s="83"/>
       <c r="M38" s="69"/>
-      <c r="N38" s="74"/>
+      <c r="N38" s="146"/>
       <c r="O38" s="71">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2481,22 +2477,22 @@
       <c r="A39" s="9"/>
       <c r="B39" s="3"/>
       <c r="C39" s="1"/>
-      <c r="D39" s="85"/>
-      <c r="E39" s="85"/>
-      <c r="F39" s="85"/>
-      <c r="G39" s="85"/>
-      <c r="H39" s="85"/>
-      <c r="I39" s="85"/>
-      <c r="J39" s="85"/>
-      <c r="K39" s="85"/>
-      <c r="L39" s="85"/>
+      <c r="D39" s="142"/>
+      <c r="E39" s="142"/>
+      <c r="F39" s="142"/>
+      <c r="G39" s="142"/>
+      <c r="H39" s="142"/>
+      <c r="I39" s="142"/>
+      <c r="J39" s="142"/>
+      <c r="K39" s="142"/>
+      <c r="L39" s="142"/>
       <c r="M39" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="N39" s="75" t="s">
+      <c r="N39" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="O39" s="76">
+      <c r="O39" s="74">
         <f>SUM(O23:O38)</f>
         <v>0</v>
       </c>
@@ -2508,19 +2504,19 @@
       <c r="C40" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D40" s="86" t="s">
+      <c r="D40" s="143" t="s">
         <v>45</v>
       </c>
-      <c r="E40" s="86"/>
-      <c r="F40" s="86"/>
-      <c r="G40" s="86"/>
-      <c r="H40" s="86"/>
-      <c r="I40" s="86"/>
-      <c r="J40" s="86"/>
-      <c r="K40" s="86"/>
-      <c r="L40" s="86"/>
+      <c r="E40" s="143"/>
+      <c r="F40" s="143"/>
+      <c r="G40" s="143"/>
+      <c r="H40" s="143"/>
+      <c r="I40" s="143"/>
+      <c r="J40" s="143"/>
+      <c r="K40" s="143"/>
+      <c r="L40" s="143"/>
       <c r="M40" s="2"/>
-      <c r="N40" s="77" t="s">
+      <c r="N40" s="75" t="s">
         <v>25</v>
       </c>
       <c r="O40" s="71">
@@ -2542,7 +2538,7 @@
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
       <c r="M41" s="45"/>
-      <c r="N41" s="77" t="s">
+      <c r="N41" s="75" t="s">
         <v>26</v>
       </c>
       <c r="O41" s="71">
@@ -2566,10 +2562,10 @@
       <c r="K42" s="5"/>
       <c r="L42" s="5"/>
       <c r="M42" s="45"/>
-      <c r="N42" s="78" t="s">
+      <c r="N42" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="O42" s="79">
+      <c r="O42" s="77">
         <f>SUM(O39:O41)</f>
         <v>0</v>
       </c>
@@ -2577,19 +2573,19 @@
     </row>
     <row r="43" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="9"/>
-      <c r="B43" s="83" t="s">
+      <c r="B43" s="144" t="s">
         <v>32</v>
       </c>
-      <c r="C43" s="83"/>
-      <c r="D43" s="84"/>
-      <c r="E43" s="84"/>
-      <c r="F43" s="84"/>
-      <c r="G43" s="84"/>
-      <c r="H43" s="84"/>
-      <c r="I43" s="84"/>
-      <c r="J43" s="84"/>
-      <c r="K43" s="84"/>
-      <c r="L43" s="84"/>
+      <c r="C43" s="144"/>
+      <c r="D43" s="145"/>
+      <c r="E43" s="145"/>
+      <c r="F43" s="145"/>
+      <c r="G43" s="145"/>
+      <c r="H43" s="145"/>
+      <c r="I43" s="145"/>
+      <c r="J43" s="145"/>
+      <c r="K43" s="145"/>
+      <c r="L43" s="145"/>
       <c r="M43" s="46" t="s">
         <v>27</v>
       </c>
@@ -2597,19 +2593,19 @@
     </row>
     <row r="44" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="9"/>
-      <c r="B44" s="83" t="s">
+      <c r="B44" s="144" t="s">
         <v>33</v>
       </c>
-      <c r="C44" s="83"/>
-      <c r="D44" s="84"/>
-      <c r="E44" s="84"/>
-      <c r="F44" s="84"/>
-      <c r="G44" s="84"/>
-      <c r="H44" s="84"/>
-      <c r="I44" s="84"/>
-      <c r="J44" s="84"/>
-      <c r="K44" s="84"/>
-      <c r="L44" s="84"/>
+      <c r="C44" s="144"/>
+      <c r="D44" s="145"/>
+      <c r="E44" s="145"/>
+      <c r="F44" s="145"/>
+      <c r="G44" s="145"/>
+      <c r="H44" s="145"/>
+      <c r="I44" s="145"/>
+      <c r="J44" s="145"/>
+      <c r="K44" s="145"/>
+      <c r="L44" s="145"/>
       <c r="M44" s="46" t="s">
         <v>16</v>
       </c>
@@ -2618,38 +2614,38 @@
       <c r="P44" s="43"/>
     </row>
     <row r="45" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="83" t="s">
+      <c r="B45" s="144" t="s">
         <v>36</v>
       </c>
-      <c r="C45" s="83"/>
-      <c r="D45" s="84"/>
-      <c r="E45" s="84"/>
-      <c r="F45" s="84"/>
-      <c r="G45" s="84"/>
-      <c r="H45" s="84"/>
-      <c r="I45" s="84"/>
-      <c r="J45" s="84"/>
-      <c r="K45" s="84"/>
-      <c r="L45" s="84"/>
+      <c r="C45" s="144"/>
+      <c r="D45" s="145"/>
+      <c r="E45" s="145"/>
+      <c r="F45" s="145"/>
+      <c r="G45" s="145"/>
+      <c r="H45" s="145"/>
+      <c r="I45" s="145"/>
+      <c r="J45" s="145"/>
+      <c r="K45" s="145"/>
+      <c r="L45" s="145"/>
       <c r="M45" s="46" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
-      <c r="B46" s="83" t="s">
+      <c r="B46" s="144" t="s">
         <v>34</v>
       </c>
-      <c r="C46" s="83"/>
-      <c r="D46" s="84"/>
-      <c r="E46" s="84"/>
-      <c r="F46" s="84"/>
-      <c r="G46" s="84"/>
-      <c r="H46" s="84"/>
-      <c r="I46" s="84"/>
-      <c r="J46" s="84"/>
-      <c r="K46" s="84"/>
-      <c r="L46" s="84"/>
+      <c r="C46" s="144"/>
+      <c r="D46" s="145"/>
+      <c r="E46" s="145"/>
+      <c r="F46" s="145"/>
+      <c r="G46" s="145"/>
+      <c r="H46" s="145"/>
+      <c r="I46" s="145"/>
+      <c r="J46" s="145"/>
+      <c r="K46" s="145"/>
+      <c r="L46" s="145"/>
       <c r="M46" s="46" t="s">
         <v>17</v>
       </c>
@@ -2658,11 +2654,49 @@
   </sheetData>
   <sheetProtection password="C7D5" sheet="1" objects="1" scenarios="1" formatCells="0"/>
   <mergeCells count="63">
-    <mergeCell ref="C24:L24"/>
-    <mergeCell ref="C23:L23"/>
-    <mergeCell ref="C25:L25"/>
-    <mergeCell ref="C26:L26"/>
-    <mergeCell ref="C27:L27"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:L44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:L45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:L46"/>
+    <mergeCell ref="D39:L39"/>
+    <mergeCell ref="D40:L40"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:L43"/>
+    <mergeCell ref="C38:L38"/>
+    <mergeCell ref="C33:L33"/>
+    <mergeCell ref="C34:L34"/>
+    <mergeCell ref="C35:L35"/>
+    <mergeCell ref="C36:L36"/>
+    <mergeCell ref="C37:L37"/>
+    <mergeCell ref="C28:L28"/>
+    <mergeCell ref="C29:L29"/>
+    <mergeCell ref="C30:L30"/>
+    <mergeCell ref="C31:L31"/>
+    <mergeCell ref="C32:L32"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="J20:O20"/>
+    <mergeCell ref="C22:L22"/>
+    <mergeCell ref="F18:O18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="Q14:V14"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="L15:O15"/>
+    <mergeCell ref="Q15:V15"/>
+    <mergeCell ref="C16:L16"/>
+    <mergeCell ref="C17:L17"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="L12:O12"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="L13:O13"/>
+    <mergeCell ref="B14:H14"/>
+    <mergeCell ref="L14:O14"/>
     <mergeCell ref="Q11:V11"/>
     <mergeCell ref="C1:N1"/>
     <mergeCell ref="C2:N2"/>
@@ -2678,49 +2712,11 @@
     <mergeCell ref="L10:N10"/>
     <mergeCell ref="B11:H11"/>
     <mergeCell ref="L11:O11"/>
-    <mergeCell ref="C17:L17"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="L12:O12"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="L13:O13"/>
-    <mergeCell ref="B14:H14"/>
-    <mergeCell ref="L14:O14"/>
-    <mergeCell ref="Q14:V14"/>
-    <mergeCell ref="B15:H15"/>
-    <mergeCell ref="L15:O15"/>
-    <mergeCell ref="Q15:V15"/>
-    <mergeCell ref="C16:L16"/>
-    <mergeCell ref="F18:O18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="J20:O20"/>
-    <mergeCell ref="C22:L22"/>
-    <mergeCell ref="C28:L28"/>
-    <mergeCell ref="C29:L29"/>
-    <mergeCell ref="C30:L30"/>
-    <mergeCell ref="C31:L31"/>
-    <mergeCell ref="C32:L32"/>
-    <mergeCell ref="C33:L33"/>
-    <mergeCell ref="C34:L34"/>
-    <mergeCell ref="C35:L35"/>
-    <mergeCell ref="C36:L36"/>
-    <mergeCell ref="C37:L37"/>
-    <mergeCell ref="D39:L39"/>
-    <mergeCell ref="D40:L40"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:L43"/>
-    <mergeCell ref="C38:L38"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:L44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:L45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:L46"/>
+    <mergeCell ref="C24:L24"/>
+    <mergeCell ref="C23:L23"/>
+    <mergeCell ref="C25:L25"/>
+    <mergeCell ref="C26:L26"/>
+    <mergeCell ref="C27:L27"/>
   </mergeCells>
   <pageMargins left="0.45" right="0.42" top="0.34" bottom="0.27" header="0.17" footer="0.17"/>
   <pageSetup scale="87" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>